<commit_message>
Extra plots for TOX21
</commit_message>
<xml_diff>
--- a/ExperimentList/tox21_combinations.xlsx
+++ b/ExperimentList/tox21_combinations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaspertl/Library/Mobile Documents/com~apple~CloudDocs/Cambridge part III/Project/CompleteCodeGit/ExperimentList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DC55730-6E96-4740-925D-55B7C82D015F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA1B1472-7781-7E45-AE31-E6D93A558E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="760" windowWidth="29400" windowHeight="17080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
     <t>28, 28, 28</t>
   </si>
   <si>
-    <t>12, 12, 12, 12, 12</t>
+    <t>12, 12, 9</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>